<commit_message>
November update, pull_tables updated
</commit_message>
<xml_diff>
--- a/Klinisk/Mammary tumor patients.xlsx
+++ b/Klinisk/Mammary tumor patients.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10918"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jqc305/Documents/PhD/Klinisk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E099564-2DF7-4244-9E14-48E225EBF40D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E099564-2DF7-4244-9E14-48E225EBF40D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{05FC4E04-0877-594A-B04F-0D4C4ACDAED3}"/>
   </bookViews>
@@ -17,13 +17,21 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
     <sheet name="For Kerstin" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1708,7 +1716,7 @@
     <filterColumn colId="16" hiddenButton="1"/>
     <filterColumn colId="17" hiddenButton="1"/>
   </autoFilter>
-  <sortState ref="A2:R21">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R21">
     <sortCondition ref="I6"/>
   </sortState>
   <tableColumns count="18">
@@ -2036,7 +2044,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2050,12 +2058,12 @@
       <selection activeCell="A4" sqref="A4:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.93359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.80859375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2202,26 +2210,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E1C8720-BEBF-7D49-9996-CB1A7CAFC779}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="117" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.1640625" customWidth="1"/>
+    <col min="1" max="1" width="15.53515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.87890625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.2734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.93359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.2734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.0078125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.62890625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.1484375" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="13" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="10.8515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.35546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="11.34375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.9921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2556,7 +2564,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>30</v>
       </c>
@@ -2752,7 +2760,7 @@
       <c r="Q10" s="11"/>
       <c r="R10" s="11"/>
     </row>
-    <row r="11" spans="1:18" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>63</v>
       </c>
@@ -2968,7 +2976,7 @@
       </c>
       <c r="R14" s="11"/>
     </row>
-    <row r="15" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>66</v>
       </c>
@@ -3024,7 +3032,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>109</v>
       </c>
@@ -3064,7 +3072,7 @@
       <c r="Q16" s="29"/>
       <c r="R16" s="11"/>
     </row>
-    <row r="17" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>54</v>
       </c>
@@ -3318,11 +3326,11 @@
       <c r="Q21" s="29"/>
       <c r="R21" s="11"/>
     </row>
-    <row r="22" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>57</v>
       </c>
@@ -3367,7 +3375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>62</v>
       </c>
@@ -3459,7 +3467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D31" s="47" t="s">
         <v>85</v>
       </c>
@@ -3474,7 +3482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="J32" t="s">
@@ -3549,7 +3557,7 @@
       </c>
       <c r="F38" s="51"/>
     </row>
-    <row r="39" spans="4:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D39" s="47" t="s">
         <v>85</v>
       </c>
@@ -3559,7 +3567,7 @@
       </c>
       <c r="F39" s="52"/>
     </row>
-    <row r="40" spans="4:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
     </row>
@@ -3633,7 +3641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="4:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D49" s="47" t="s">
         <v>85</v>
       </c>
@@ -3642,8 +3650,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="4:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="4:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D51" s="38" t="s">
         <v>91</v>
       </c>
@@ -3652,7 +3660,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="4:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="4:6" x14ac:dyDescent="0.2">
       <c r="D53" s="36" t="s">
         <v>98</v>
@@ -3690,7 +3698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="4:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D56" s="34" t="s">
         <v>97</v>
       </c>
@@ -3704,7 +3712,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="J24:K31">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J24:K31">
     <sortCondition ref="J24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>